<commit_message>
updated data for race estimates
</commit_message>
<xml_diff>
--- a/src/dashboard/Data/Indicators.xlsx
+++ b/src/dashboard/Data/Indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myuva.sharepoint.com/sites/DSPG20203-State/Shared Documents/UVA-Gates-Wasco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="543" documentId="13_ncr:1_{12818DC3-1CB4-D44B-85AC-EFEAE5EC3816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5CD3A671-5D35-6D41-A897-F2938B4BE4EE}"/>
+  <xr:revisionPtr revIDLastSave="546" documentId="13_ncr:1_{12818DC3-1CB4-D44B-85AC-EFEAE5EC3816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E0FE0891-5CE8-D740-9124-C67CA3F6FEC1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33720" windowHeight="16120" activeTab="2" xr2:uid="{2542D41E-D2EC-EF44-9353-0EB32E186B84}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" activeTab="3" xr2:uid="{2542D41E-D2EC-EF44-9353-0EB32E186B84}"/>
   </bookViews>
   <sheets>
     <sheet name="Infrastructure" sheetId="2" r:id="rId1"/>
@@ -36,35 +36,110 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="145">
+  <si>
+    <t>Cluster: Infrastructure</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Indicator</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Datasource</t>
+  </si>
+  <si>
+    <t>Geographic Level</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Years Collected</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>Broadband</t>
+  </si>
+  <si>
+    <t>Access to broadband fosters business innovation, education, and economic opportunity</t>
+  </si>
+  <si>
+    <t>% Households with access to broadband, Funding for broadband</t>
+  </si>
+  <si>
+    <t>ACS / Oregon Broadband Office</t>
+  </si>
+  <si>
+    <t>County, census block and school district</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>info card being created</t>
+  </si>
+  <si>
+    <t>Water/Wastewater</t>
+  </si>
+  <si>
+    <t>Good water quality is essential to human health, social and economic development, and the ecosystem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average cost &amp; gallons of water treated vs gallons of water used daily </t>
+  </si>
+  <si>
+    <t>Oregon's water use tool</t>
+  </si>
+  <si>
+    <t>By entity or Facility</t>
+  </si>
+  <si>
+    <t>Wind &amp; Solar Energy</t>
+  </si>
+  <si>
+    <t>"For every megawatt of wind capacity installed from 2000 to 2008, annual total personal income rose by approximately $11,000, and 0.5 jobs were created"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average cost per project and projected profits </t>
+  </si>
+  <si>
+    <t>Financial Analysis of projects</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Cities that facilitate multi-modal transportation are able to bring in more talent</t>
+  </si>
+  <si>
+    <t>Average cost &amp; how many bus stops in S. Wasco</t>
+  </si>
+  <si>
+    <t>Wasco Bus maps</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
   <si>
     <t>Cluster: Food Systems</t>
   </si>
   <si>
-    <t>Domain</t>
-  </si>
-  <si>
-    <t>Indicator</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Metric</t>
-  </si>
-  <si>
-    <t>Datasource</t>
-  </si>
-  <si>
-    <t>Geographic Level</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>Food</t>
   </si>
   <si>
@@ -74,15 +149,15 @@
     <t>Grocery store and locally grown food access</t>
   </si>
   <si>
+    <t>location and frequency of grocery stores and food businesses in the area</t>
+  </si>
+  <si>
     <t>Oregon Live, USDA Local Food Directory</t>
   </si>
   <si>
     <t xml:space="preserve">County </t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>ACS = American Community Survey</t>
   </si>
   <si>
@@ -95,148 +170,190 @@
     <t>Unemployment + Poverty + Median Income + % Hispanic + % Black + % Homeowners + % Individuals with Disability</t>
   </si>
   <si>
+    <t>Feeding America Map the Meal Gap</t>
+  </si>
+  <si>
+    <t>county, state, school district</t>
+  </si>
+  <si>
+    <t>1 year estimates for state level &amp; 5year estimates at the county level</t>
+  </si>
+  <si>
+    <t>2015-2019</t>
+  </si>
+  <si>
     <t>BLS = Bureau of Labor Statistics</t>
   </si>
   <si>
+    <t>WIC Acceptance</t>
+  </si>
+  <si>
+    <t>The special supplemental nutrition program for Women, Infants, and Children (WIC) is a federally funded program designed to target food insecure new mothers and children</t>
+  </si>
+  <si>
+    <t># of stores accepting WIC in area</t>
+  </si>
+  <si>
+    <t>Oregon Health Authority</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>HRSA = Health Resources and Services Administration</t>
+  </si>
+  <si>
+    <t>SNAP Acceptance</t>
+  </si>
+  <si>
+    <t>The Supplemental Nutrition Assistance Program (SNAP) is a federally funded program designed to target food insecure low-income individuals and families.</t>
+  </si>
+  <si>
+    <t># of stores accepting SNAP in area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USDA </t>
+  </si>
+  <si>
+    <t>LEHD-LODES=LEHD Origin-Destination Employment Statistics</t>
+  </si>
+  <si>
+    <t>Driver: Opportunities to Learn and Earn</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>College preparedness</t>
+  </si>
+  <si>
+    <t>A student who withdrew and did not graduate or transfer to another school that leads to graduation. This excludes students who leave and receive GED certificate.</t>
+  </si>
+  <si>
+    <t>High school dropout rate</t>
+  </si>
+  <si>
+    <t>Oregon Department of Education: Droput Rate Data</t>
+  </si>
+  <si>
     <t>school district</t>
   </si>
   <si>
+    <t>1 school year</t>
+  </si>
+  <si>
+    <t>2014-2018</t>
+  </si>
+  <si>
+    <t>Students who graduate within four years of entering high school</t>
+  </si>
+  <si>
+    <t>On-Time Graduation</t>
+  </si>
+  <si>
+    <t>Oregon Department of Education: Report Card Data</t>
+  </si>
+  <si>
+    <t>Quality of Public Education</t>
+  </si>
+  <si>
+    <t>Higher rates of improvement in English Language Arts indicate more effective public education (Urban Institute)</t>
+  </si>
+  <si>
+    <t>Average per-grade change in English Language Arts achievement between third and eigth grades (Urban Institute)</t>
+  </si>
+  <si>
+    <t>Oregon Department of Education: English Language Arts Assessment Reports</t>
+  </si>
+  <si>
+    <t>% of certified teachers who have taught for 3 or more years in oregon or in other states.</t>
+  </si>
+  <si>
+    <t>% Teacher Experience</t>
+  </si>
+  <si>
+    <t>2014, 2015, 2018</t>
+  </si>
+  <si>
+    <t>inconsistent across years</t>
+  </si>
+  <si>
+    <t>Chronic Absenteeism</t>
+  </si>
+  <si>
+    <t>Students with regular attendance are more likely to succeed (better chance of economic mobility) (Urban Institute)</t>
+  </si>
+  <si>
+    <t>% of students who are absent on 10% or more of the school days they are enrolled in for a school year.</t>
+  </si>
+  <si>
+    <t>Oregon Department of Education: Regular Attenders Report</t>
+  </si>
+  <si>
+    <t>Employment</t>
+  </si>
+  <si>
+    <t>Employment Ratio</t>
+  </si>
+  <si>
+    <t>The civilian noninstitutional population age 20-64 who are employed divided by the total civilian noninstitutional population 20 to 64 years old.</t>
+  </si>
+  <si>
+    <t>Employment to population ratio for adults ages 20-64</t>
+  </si>
+  <si>
+    <t>ACS: S2301</t>
+  </si>
+  <si>
+    <t>County, census tract, school district</t>
+  </si>
+  <si>
+    <t>1year &amp; 5 year est.</t>
+  </si>
+  <si>
+    <t>2015-2018</t>
+  </si>
+  <si>
+    <t>Labor Force Participation Rate</t>
+  </si>
+  <si>
+    <t>Labor force includes all people classified in the civilian labor force in addition to members of the U.S. Armed Forces. Civilian labor force consists of employed or unemployed people.</t>
+  </si>
+  <si>
+    <t>Proportion of adults 20-64 in the civilian labor force</t>
+  </si>
+  <si>
+    <t>5 year estimates</t>
+  </si>
+  <si>
+    <t>Jobs per Industry</t>
+  </si>
+  <si>
+    <t>Profile of jobs per industry, such as Manufacturing, Agriculture, Education, and Healthcare.</t>
+  </si>
+  <si>
+    <t>Number of jobs in specified industry for a given geographical area</t>
+  </si>
+  <si>
+    <t>LEHD-LODES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">County, census block </t>
+  </si>
+  <si>
     <t>1 year</t>
   </si>
   <si>
-    <t>WIC Acceptance</t>
-  </si>
-  <si>
-    <t>The special supplemental nutrition program for Women, Infants, and Children (WIC) is a federally funded program designed to target food insecure new mothers and children</t>
-  </si>
-  <si>
-    <t># of stores accepting WIC in area</t>
-  </si>
-  <si>
-    <t>Oregon Health Authority</t>
-  </si>
-  <si>
-    <t>Place</t>
-  </si>
-  <si>
-    <t>HRSA = Health Resources and Services Administration</t>
-  </si>
-  <si>
-    <t>SNAP Acceptance</t>
-  </si>
-  <si>
-    <t>The Supplemental Nutrition Assistance Program (SNAP) is a federally funded program designed to target food insecure low-income individuals and families.</t>
-  </si>
-  <si>
-    <t># of stores accepting SNAP in area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USDA </t>
-  </si>
-  <si>
-    <t>LEHD-LODES=LEHD Origin-Destination Employment Statistics</t>
-  </si>
-  <si>
-    <t>Cluster: Infrastructure</t>
-  </si>
-  <si>
-    <t>Infrastructure</t>
-  </si>
-  <si>
-    <t>Broadband</t>
-  </si>
-  <si>
-    <t>Access to broadband fosters business innovation, education, and economic opportunity</t>
-  </si>
-  <si>
-    <t>ACS / Oregon Broadband Office</t>
-  </si>
-  <si>
-    <t>County, census block and school district</t>
-  </si>
-  <si>
-    <t>Water/Wastewater</t>
-  </si>
-  <si>
-    <t>Good water quality is essential to human health, social and economic development, and the ecosystem.</t>
-  </si>
-  <si>
-    <t>Oregon's water use tool</t>
-  </si>
-  <si>
-    <t>By entity or Facility</t>
-  </si>
-  <si>
-    <t>Wind &amp; Solar Energy</t>
-  </si>
-  <si>
-    <t>"For every megawatt of wind capacity installed from 2000 to 2008, annual total personal income rose by approximately $11,000, and 0.5 jobs were created"</t>
-  </si>
-  <si>
-    <t>Financial Analysis of projects</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>Cities that facilitate multi-modal transportation are able to bring in more talent</t>
-  </si>
-  <si>
-    <t>Wasco Bus maps</t>
-  </si>
-  <si>
-    <t>Driver: Opportunities to Learn and Earn</t>
-  </si>
-  <si>
-    <t>Education</t>
-  </si>
-  <si>
-    <t>College preparedness</t>
-  </si>
-  <si>
-    <t>Quality of Public Education</t>
-  </si>
-  <si>
-    <t>Higher rates of improvement in English Language Arts indicate more effective public education (Urban Institute)</t>
-  </si>
-  <si>
-    <t>Average per-grade change in English Language Arts achievement between third and eigth grades (Urban Institute)</t>
-  </si>
-  <si>
-    <t>% of certified teachers who have taught for 3 or more years in oregon or in other states.</t>
-  </si>
-  <si>
-    <t>% Teacher Experience</t>
-  </si>
-  <si>
-    <t>Chronic Absenteeism</t>
-  </si>
-  <si>
-    <t>Students with regular attendance are more likely to succeed (better chance of economic mobility) (Urban Institute)</t>
-  </si>
-  <si>
-    <t>% of students who are absent on 10% or more of the school days they are enrolled in for a school year.</t>
-  </si>
-  <si>
-    <t>Employment</t>
-  </si>
-  <si>
-    <t>Employment Ratio</t>
-  </si>
-  <si>
-    <t>1year &amp; 5 year est.</t>
-  </si>
-  <si>
-    <t>Jobs per Industry</t>
-  </si>
-  <si>
-    <t>Profile of jobs per industry, such as Manufacturing, Agriculture, Education, and Healthcare.</t>
-  </si>
-  <si>
-    <t>Number of jobs in specified industry for a given geographical area</t>
-  </si>
-  <si>
-    <t>LEHD-LODES</t>
+    <t>2015-2017</t>
+  </si>
+  <si>
+    <t>Worker inflows and outflows</t>
+  </si>
+  <si>
+    <t>inflows: number of employees from each county traveling into the region for work. Outflows are the number of workers from the region traveling out to other counties for work</t>
+  </si>
+  <si>
+    <t>Number of workers per county</t>
   </si>
   <si>
     <t>Driver: Quality Standard of Living</t>
@@ -251,10 +368,46 @@
     <t xml:space="preserve">Income at the household level determines if basic needs can be met. </t>
   </si>
   <si>
+    <t>Median Household Income</t>
+  </si>
+  <si>
+    <t>ACS: S1901</t>
+  </si>
+  <si>
+    <t>5 year estimate</t>
+  </si>
+  <si>
+    <t>Income Distribution</t>
+  </si>
+  <si>
+    <t>% of Population for each Income bracket</t>
+  </si>
+  <si>
+    <t>6 year estimate</t>
+  </si>
+  <si>
     <t>Poverty Rate</t>
   </si>
   <si>
-    <t>%of population for whom poverty status is determined.</t>
+    <t xml:space="preserve">% Below Federal Poverty </t>
+  </si>
+  <si>
+    <t>ALICE Households</t>
+  </si>
+  <si>
+    <t>% of ALICE Households</t>
+  </si>
+  <si>
+    <t>United for ALICE</t>
+  </si>
+  <si>
+    <t>County, place</t>
+  </si>
+  <si>
+    <t>2 year estimates for county 5 year estimates for place</t>
+  </si>
+  <si>
+    <t>2010-2018</t>
   </si>
   <si>
     <t>Housing</t>
@@ -266,6 +419,21 @@
     <t xml:space="preserve">The security of affordable housing allows for the household budget to be able to pay for other basic needs such as food, health care, and education. </t>
   </si>
   <si>
+    <t>ratio of affordable (monthly costs are less than or equal to 30% of a household's income) housing units to occupied houses.</t>
+  </si>
+  <si>
+    <t>ACS: B25106</t>
+  </si>
+  <si>
+    <t>Homeownership Rate</t>
+  </si>
+  <si>
+    <t>% of Homes occupied by Homeowner</t>
+  </si>
+  <si>
+    <t>ACS: B25003</t>
+  </si>
+  <si>
     <t>Social</t>
   </si>
   <si>
@@ -284,190 +452,25 @@
     <t>Household with two married parents is a predictor of intergenerational upward mobility (Chetty)</t>
   </si>
   <si>
+    <t xml:space="preserve">Household type with own children under 18 </t>
+  </si>
+  <si>
+    <t>ACS: B09005</t>
+  </si>
+  <si>
     <t>Education Level</t>
   </si>
   <si>
     <t>Highest degree obtained for population 25 years and older</t>
   </si>
   <si>
-    <t>High school dropout rate</t>
-  </si>
-  <si>
-    <t>On-Time Graduation</t>
-  </si>
-  <si>
-    <t>Average cost &amp; how many bus stops in S. Wasco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average cost &amp; gallons of water treated vs gallons of water used daily </t>
-  </si>
-  <si>
-    <t>County</t>
-  </si>
-  <si>
-    <t>county</t>
-  </si>
-  <si>
-    <t>info card being created</t>
-  </si>
-  <si>
-    <t>county, state, school district</t>
-  </si>
-  <si>
-    <t>2015-2018</t>
-  </si>
-  <si>
-    <t>2015-2019</t>
-  </si>
-  <si>
-    <t>Years Collected</t>
-  </si>
-  <si>
-    <t>inconsistent across years</t>
-  </si>
-  <si>
-    <t>1 school year</t>
-  </si>
-  <si>
-    <t>2015-2017</t>
-  </si>
-  <si>
-    <t>2014-2018</t>
-  </si>
-  <si>
-    <t>2014, 2015, 2018</t>
-  </si>
-  <si>
-    <t>Labor Force Participation Rate</t>
-  </si>
-  <si>
-    <t>Employment to population ratio for adults ages 20-64</t>
-  </si>
-  <si>
-    <t>Labor force includes all people classified in the civilian labor force in addition to members of the U.S. Armed Forces. Civilian labor force consists of employed or unemployed people.</t>
-  </si>
-  <si>
-    <t>Proportion of adults 20-64 in the civilian labor force</t>
-  </si>
-  <si>
-    <t>County, census tract, school district</t>
-  </si>
-  <si>
-    <t>5 year estimates</t>
-  </si>
-  <si>
-    <t>Students who graduate within four years of entering high school</t>
-  </si>
-  <si>
-    <t>ALICE Households</t>
-  </si>
-  <si>
-    <t>United for ALICE</t>
-  </si>
-  <si>
-    <t>County, place</t>
-  </si>
-  <si>
-    <t>2 year estimates for county 5 year estimates for place</t>
-  </si>
-  <si>
-    <t>2010-2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average cost per project and projected profits </t>
-  </si>
-  <si>
-    <t>% Households with access to broadband, Funding for broadband</t>
-  </si>
-  <si>
-    <t>% of ALICE Households</t>
-  </si>
-  <si>
-    <t>Homeownership Rate</t>
-  </si>
-  <si>
-    <t>% of Homes occupied by Homeowner</t>
-  </si>
-  <si>
-    <t>5 year estimate</t>
-  </si>
-  <si>
-    <t>A student who withdrew and did not graduate or transfer to another school that leads to graduation. This excludes students who leave and receive GED certificate.</t>
-  </si>
-  <si>
-    <t>Oregon Department of Education: Droput Rate Data</t>
-  </si>
-  <si>
-    <t>Oregon Department of Education: English Language Arts Assessment Reports</t>
-  </si>
-  <si>
-    <t>Oregon Department of Education: Regular Attenders Report</t>
-  </si>
-  <si>
-    <t>Oregon Department of Education: Report Card Data</t>
-  </si>
-  <si>
-    <t>Feeding America Map the Meal Gap</t>
-  </si>
-  <si>
-    <t>1 year estimates for state level &amp; 5year estimates at the county level</t>
-  </si>
-  <si>
-    <t>location and frequency of grocery stores and food businesses in the area</t>
-  </si>
-  <si>
-    <t>Worker inflows and outflows</t>
-  </si>
-  <si>
-    <t>inflows: number of employees from each county traveling into the region for work. Outflows are the number of workers from the region traveling out to other counties for work</t>
-  </si>
-  <si>
-    <t>Number of workers per county</t>
-  </si>
-  <si>
-    <t xml:space="preserve">County, census block </t>
-  </si>
-  <si>
-    <t>The civilian noninstitutional population age 20-64 who are employed divided by the total civilian noninstitutional population 20 to 64 years old.</t>
-  </si>
-  <si>
-    <t>Median Household Income</t>
-  </si>
-  <si>
-    <t>% of Population for each Income bracket</t>
-  </si>
-  <si>
-    <t>Income Distribution</t>
-  </si>
-  <si>
-    <t>6 year estimate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Household type with own children under 18 </t>
-  </si>
-  <si>
-    <t>ACS: S1901</t>
-  </si>
-  <si>
-    <t>ACS: B09005</t>
-  </si>
-  <si>
-    <t>ACS: B25003</t>
-  </si>
-  <si>
-    <t>ACS: B25106</t>
-  </si>
-  <si>
     <t>ACS: S1501</t>
   </si>
   <si>
-    <t>ACS: S2301</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% Below Federal Poverty </t>
-  </si>
-  <si>
-    <t>ratio of affordable (monthly costs are less than or equal to 30% of a household's income) housing units to occupied houses.</t>
+    <t>% of population for whom poverty status is determined on the federal level.</t>
+  </si>
+  <si>
+    <t>ALICE is an acronym for Asset Limited Income Constrained, Employed. These are households that earn above the Federal Poverty Level, but not enough to afford a 'bare-bones' household budget</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1043,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="35" customHeight="1" thickBot="1">
       <c r="A1" s="15" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -1076,117 +1079,117 @@
         <v>7</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="102">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="106" customHeight="1">
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="139" customHeight="1">
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>112</v>
+        <v>25</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="98" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1224,7 +1227,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="52" customHeight="1" thickBot="1">
       <c r="A1" s="15" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -1259,119 +1262,119 @@
         <v>7</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" s="6"/>
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" ht="34">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>125</v>
+        <v>37</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="68">
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>124</v>
+        <v>46</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="118" customHeight="1">
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L5" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="91" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L6" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1393,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BC0FA8-31CF-7F43-881D-8C47CCDBDAF4}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1409,7 +1412,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="40" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -1443,230 +1446,230 @@
         <v>7</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="115" customHeight="1">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>119</v>
+        <v>65</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:10" ht="107" customHeight="1">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:10" ht="106" customHeight="1">
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:10" ht="119" customHeight="1">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="119" customHeight="1">
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="120" customHeight="1">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>141</v>
+        <v>88</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" ht="120" customHeight="1">
       <c r="B9" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>141</v>
+        <v>88</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" ht="51">
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" ht="127" customHeight="1">
       <c r="B11" s="1" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1689,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017DB1EB-0AE3-E348-82D1-EF1F8768F175}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1705,7 +1708,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="49" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -1739,224 +1742,226 @@
         <v>7</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="51">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="50" customHeight="1">
       <c r="B4" s="1" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="96" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>118</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="D6" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="113" customHeight="1">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="113" customHeight="1">
       <c r="B8" s="1" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="80" customHeight="1">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>79</v>
+        <v>135</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="86" customHeight="1">
       <c r="B10" s="1" t="s">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="34">
       <c r="B11" s="1" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -1992,6 +1997,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F4C7EABC70075D478B747307275858D0" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="87112c42fa20847ffdaa2dcf1f294382">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8b84ec8a-a026-44fa-8a36-37fd9b34b733" xmlns:ns3="c2922497-efa2-49d8-8f2a-b8a322d29f44" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a5e406d4643ea691fc87860beef6454" ns2:_="" ns3:_="">
     <xsd:import namespace="8b84ec8a-a026-44fa-8a36-37fd9b34b733"/>
@@ -2208,22 +2228,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CCD999B-BE49-454A-B160-404FA1560D18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8b84ec8a-a026-44fa-8a36-37fd9b34b733"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c2922497-efa2-49d8-8f2a-b8a322d29f44"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B64C1B8F-7B33-4306-89AD-852442027FE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B385343D-82C0-416A-A256-F383E8FAF39A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2240,29 +2270,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B64C1B8F-7B33-4306-89AD-852442027FE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CCD999B-BE49-454A-B160-404FA1560D18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c2922497-efa2-49d8-8f2a-b8a322d29f44"/>
-    <ds:schemaRef ds:uri="8b84ec8a-a026-44fa-8a36-37fd9b34b733"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>